<commit_message>
test: enhance fare calculation logic, improve error handling, and add comprehensive unit tests
</commit_message>
<xml_diff>
--- a/src/main/kotlin/config/tariff_V1.xlsx
+++ b/src/main/kotlin/config/tariff_V1.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10720"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11102"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arismendi/Documents/personal/Command-Line-Fare-Calculator/src/main/kotlin/config/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7AE1CD6-B14C-1743-9125-E9784B0D8154}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCC6EFF7-DDC4-B742-84E9-69204B177B17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -613,7 +613,7 @@
   <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -883,7 +883,7 @@
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -954,16 +954,16 @@
         <v>8</v>
       </c>
       <c r="D3" s="4">
+        <v>10</v>
+      </c>
+      <c r="E3" s="4">
         <v>8</v>
       </c>
-      <c r="E3" s="4">
-        <v>6</v>
-      </c>
       <c r="F3" s="4">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="G3" s="4">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
@@ -977,16 +977,16 @@
         <v>16</v>
       </c>
       <c r="D4" s="4">
+        <v>20</v>
+      </c>
+      <c r="E4" s="4">
         <v>16</v>
       </c>
-      <c r="E4" s="4">
-        <v>12</v>
-      </c>
       <c r="F4" s="4">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="G4" s="4">
-        <v>8</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
@@ -1000,16 +1000,16 @@
         <v>24</v>
       </c>
       <c r="D5" s="4">
+        <v>30</v>
+      </c>
+      <c r="E5" s="4">
         <v>24</v>
       </c>
-      <c r="E5" s="4">
-        <v>18</v>
-      </c>
       <c r="F5" s="4">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="G5" s="4">
-        <v>12</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>